<commit_message>
Personality profile inference v0.2
</commit_message>
<xml_diff>
--- a/data/Average Emotion Statistics.xlsx
+++ b/data/Average Emotion Statistics.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="26">
   <si>
     <t>Dominance</t>
   </si>
@@ -58,6 +58,45 @@
   </si>
   <si>
     <t>Threshold</t>
+  </si>
+  <si>
+    <t>Dominance / Steadiness</t>
+  </si>
+  <si>
+    <t>Influence / Compliance</t>
+  </si>
+  <si>
+    <t>% of negative words / tonal words</t>
+  </si>
+  <si>
+    <t>% of surprise words / tonal words</t>
+  </si>
+  <si>
+    <t>% of fear words / tonal words</t>
+  </si>
+  <si>
+    <t>% of trust words / tonal words</t>
+  </si>
+  <si>
+    <t>% of joy words / tonal words</t>
+  </si>
+  <si>
+    <t>% of anticipation words / tonal words</t>
+  </si>
+  <si>
+    <t>% of anger words / tonal words</t>
+  </si>
+  <si>
+    <t>10% Gap</t>
+  </si>
+  <si>
+    <t>1 each way</t>
+  </si>
+  <si>
+    <t>3 each way</t>
+  </si>
+  <si>
+    <t>2 each way</t>
   </si>
 </sst>
 </file>
@@ -121,8 +160,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -167,7 +234,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -176,6 +243,20 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -184,6 +265,20 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -513,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V31"/>
+  <dimension ref="A1:V53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -745,7 +840,7 @@
         <v>4.7619047619047603E-2</v>
       </c>
       <c r="V6" s="8">
-        <f t="shared" ref="V5:V14" si="0">AVERAGE(B6:U6)</f>
+        <f t="shared" ref="V6:V14" si="0">AVERAGE(B6:U6)</f>
         <v>0.13246554128353835</v>
       </c>
     </row>
@@ -895,71 +990,71 @@
     </row>
     <row r="10" spans="1:22">
       <c r="A10" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B10">
-        <v>9.0308370044052802E-2</v>
+        <v>0.585365853658536</v>
       </c>
       <c r="C10">
-        <v>8.5271317829457294E-2</v>
+        <v>0.19191919191919099</v>
       </c>
       <c r="D10">
-        <v>7.1118349619978205E-2</v>
+        <v>0.221374045801526</v>
       </c>
       <c r="E10">
-        <v>7.3052870949403007E-2</v>
+        <v>2.7237354085603099E-2</v>
       </c>
       <c r="F10">
-        <v>8.0766995932597299E-2</v>
+        <v>0.15107913669064699</v>
       </c>
       <c r="G10">
-        <v>8.2623935903855694E-2</v>
+        <v>5.4545454545454501E-2</v>
       </c>
       <c r="H10">
-        <v>6.7348377997179104E-2</v>
+        <v>0.162303664921465</v>
       </c>
       <c r="I10">
-        <v>7.3577235772357696E-2</v>
+        <v>4.9723756906077297E-2</v>
       </c>
       <c r="J10">
-        <v>5.7561486132914702E-2</v>
+        <v>0.218181818181818</v>
       </c>
       <c r="K10">
-        <v>8.9592274678111594E-2</v>
+        <v>8.9820359281437098E-2</v>
       </c>
       <c r="L10">
-        <v>6.0206185567010302E-2</v>
+        <v>4.1095890410958902E-2</v>
       </c>
       <c r="M10">
-        <v>9.0142095914742398E-2</v>
+        <v>0.43842364532019701</v>
       </c>
       <c r="N10">
-        <v>7.5233834892232607E-2</v>
+        <v>0.26486486486486399</v>
       </c>
       <c r="O10">
-        <v>8.1927710843373497E-2</v>
+        <v>1.47058823529411E-2</v>
       </c>
       <c r="P10">
-        <v>8.5348506401137905E-2</v>
+        <v>0.266666666666666</v>
       </c>
       <c r="Q10">
-        <v>8.1067472306143001E-2</v>
+        <v>6.8322981366459604E-2</v>
       </c>
       <c r="R10">
-        <v>8.1067472306143001E-2</v>
+        <v>6.8322981366459604E-2</v>
       </c>
       <c r="S10">
-        <v>6.2363238512034999E-2</v>
+        <v>3.5087719298245598E-2</v>
       </c>
       <c r="T10">
-        <v>0.12305611899932301</v>
+        <v>1.09890109890109E-2</v>
       </c>
       <c r="U10">
-        <v>0.115279048490393</v>
+        <v>0.14285714285714199</v>
       </c>
       <c r="V10" s="8">
-        <f t="shared" si="0"/>
-        <v>8.1345644954622057E-2</v>
+        <f>AVERAGE(B10:U10)</f>
+        <v>0.15514437107423498</v>
       </c>
     </row>
     <row r="11" spans="1:22">
@@ -1178,132 +1273,593 @@
     <row r="15" spans="1:22">
       <c r="A15" s="5"/>
     </row>
+    <row r="16" spans="1:22">
+      <c r="A16" s="5"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>8.1345644954622057E-2</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0.08</v>
+      </c>
+    </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
+      <c r="A19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>0.15514437107423498</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0.16</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20">
-        <v>8.1345644954622057E-2</v>
-      </c>
-      <c r="C20" s="5">
-        <v>0.08</v>
-      </c>
+      <c r="A20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21">
-        <v>0.15514437107423498</v>
+        <v>0.13246554128353835</v>
       </c>
       <c r="C21" s="5">
-        <v>0.16</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="5"/>
+      <c r="A22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>0.10917128066888386</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0.11</v>
+      </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B23">
-        <v>0.13246554128353835</v>
+        <v>0.16116536959631694</v>
       </c>
       <c r="C23" s="5">
-        <v>0.13</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24">
-        <v>0.10917128066888386</v>
-      </c>
-      <c r="C24" s="5">
-        <v>0.11</v>
-      </c>
+      <c r="A24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B25">
-        <v>0.16116536959631694</v>
+        <v>0.15514437107423498</v>
       </c>
       <c r="C25" s="5">
         <v>0.16</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="5"/>
+      <c r="A26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26">
+        <v>0.16116536959631694</v>
+      </c>
+      <c r="C26" s="5">
+        <v>0.16</v>
+      </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>0.13246554128353835</v>
+      </c>
+      <c r="C28" s="5">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29">
+        <v>0.10053047080811524</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="6"/>
+      <c r="C30" s="5"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B27">
-        <v>8.1345644954622057E-2</v>
-      </c>
-      <c r="C27" s="5">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="4" t="s">
+      <c r="B33">
+        <v>10.726643598615899</v>
+      </c>
+      <c r="C33">
+        <v>6.3231850117096</v>
+      </c>
+      <c r="D33">
+        <v>8.5896076352067805</v>
+      </c>
+      <c r="E33">
+        <v>10.5084745762711</v>
+      </c>
+      <c r="F33">
+        <v>10.321489001691999</v>
+      </c>
+      <c r="G33">
+        <v>5.11073253833049</v>
+      </c>
+      <c r="H33">
+        <v>8.3223249669749002</v>
+      </c>
+      <c r="I33">
+        <v>4.6469523234761603</v>
+      </c>
+      <c r="J33">
+        <v>6.5664160401002496</v>
+      </c>
+      <c r="K33">
+        <v>10.2564102564102</v>
+      </c>
+      <c r="L33">
+        <f>AVERAGE(B33:K33)</f>
+        <v>8.137223594878737</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34">
+        <v>14.516129032258</v>
+      </c>
+      <c r="C34">
+        <v>39.259259259259203</v>
+      </c>
+      <c r="D34">
+        <v>41.975308641975303</v>
+      </c>
+      <c r="E34">
+        <v>19.354838709677399</v>
+      </c>
+      <c r="F34">
+        <v>18.032786885245901</v>
+      </c>
+      <c r="G34">
+        <v>70</v>
+      </c>
+      <c r="H34">
+        <v>34.920634920634903</v>
+      </c>
+      <c r="I34">
+        <v>49.350649350649299</v>
+      </c>
+      <c r="J34">
+        <v>32.824427480916</v>
+      </c>
+      <c r="K34">
+        <v>25</v>
+      </c>
+      <c r="L34">
+        <f t="shared" ref="L34:L41" si="1">AVERAGE(B34:K34)</f>
+        <v>34.523403428061599</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35">
+        <v>19.354838709677399</v>
+      </c>
+      <c r="C35">
+        <v>2.2222222222222201</v>
+      </c>
+      <c r="D35">
+        <v>9.2592592592592595</v>
+      </c>
+      <c r="E35">
+        <v>4.3010752688171996</v>
+      </c>
+      <c r="F35">
+        <v>13.114754098360599</v>
+      </c>
+      <c r="G35">
+        <v>10</v>
+      </c>
+      <c r="H35">
+        <v>3.9682539682539599</v>
+      </c>
+      <c r="I35">
+        <v>7.7922077922077904</v>
+      </c>
+      <c r="J35">
+        <v>6.1068702290076304</v>
+      </c>
+      <c r="K35">
+        <v>6.8181818181818103</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="1"/>
+        <v>8.2937663365987877</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36">
+        <v>4.8387096774193497</v>
+      </c>
+      <c r="C36">
+        <v>7.4074074074074003</v>
+      </c>
+      <c r="D36">
+        <v>9.8765432098765409</v>
+      </c>
+      <c r="E36">
+        <v>9.67741935483871</v>
+      </c>
+      <c r="F36">
+        <v>4.9180327868852398</v>
+      </c>
+      <c r="G36">
+        <v>20</v>
+      </c>
+      <c r="H36">
+        <v>8.7301587301587293</v>
+      </c>
+      <c r="I36">
+        <v>15.584415584415501</v>
+      </c>
+      <c r="J36">
+        <v>10.687022900763299</v>
+      </c>
+      <c r="K36">
+        <v>4.5454545454545396</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="1"/>
+        <v>9.6265164197219288</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38">
+        <v>4.8387096774193497</v>
+      </c>
+      <c r="C38">
+        <v>8.8888888888888893</v>
+      </c>
+      <c r="D38">
+        <v>14.1975308641975</v>
+      </c>
+      <c r="E38">
+        <v>6.4516129032257998</v>
+      </c>
+      <c r="F38">
+        <v>6.55737704918032</v>
+      </c>
+      <c r="G38">
+        <v>13.3333333333333</v>
+      </c>
+      <c r="H38">
+        <v>5.55555555555555</v>
+      </c>
+      <c r="I38">
+        <v>18.181818181818102</v>
+      </c>
+      <c r="J38">
+        <v>15.267175572518999</v>
+      </c>
+      <c r="K38">
+        <v>11.363636363636299</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="1"/>
+        <v>10.463563838977411</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39">
+        <v>27.419354838709602</v>
+      </c>
+      <c r="C39">
+        <v>10.370370370370299</v>
+      </c>
+      <c r="D39">
+        <v>14.1975308641975</v>
+      </c>
+      <c r="E39">
+        <v>16.129032258064498</v>
+      </c>
+      <c r="F39">
+        <v>18.032786885245901</v>
+      </c>
+      <c r="G39">
+        <v>10</v>
+      </c>
+      <c r="H39">
+        <v>25.396825396825299</v>
+      </c>
+      <c r="I39">
+        <v>14.285714285714199</v>
+      </c>
+      <c r="J39">
+        <v>12.9770992366412</v>
+      </c>
+      <c r="K39">
+        <v>18.181818181818102</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="1"/>
+        <v>16.699053231758661</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40">
+        <v>41.935483870967701</v>
+      </c>
+      <c r="C40">
+        <v>12.592592592592499</v>
+      </c>
+      <c r="D40">
+        <v>22.839506172839499</v>
+      </c>
+      <c r="E40">
+        <v>16.129032258064498</v>
+      </c>
+      <c r="F40">
+        <v>19.672131147540899</v>
+      </c>
+      <c r="G40">
+        <v>10</v>
+      </c>
+      <c r="H40">
+        <v>28.571428571428498</v>
+      </c>
+      <c r="I40">
+        <v>11.6883116883116</v>
+      </c>
+      <c r="J40">
+        <v>20.610687022900699</v>
+      </c>
+      <c r="K40">
+        <v>18.181818181818102</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="1"/>
+        <v>20.222099150646397</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41">
+        <v>29.0322580645161</v>
+      </c>
+      <c r="C41">
+        <v>10.370370370370299</v>
+      </c>
+      <c r="D41">
+        <v>16.049382716049301</v>
+      </c>
+      <c r="E41">
+        <v>16.129032258064498</v>
+      </c>
+      <c r="F41">
+        <v>16.393442622950801</v>
+      </c>
+      <c r="G41">
+        <v>10</v>
+      </c>
+      <c r="H41">
+        <v>22.2222222222222</v>
+      </c>
+      <c r="I41">
+        <v>11.6883116883116</v>
+      </c>
+      <c r="J41">
+        <v>13.7404580152671</v>
+      </c>
+      <c r="K41">
+        <v>18.181818181818102</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="1"/>
+        <v>16.380729613957001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45">
+        <v>8.137223594878737</v>
+      </c>
+      <c r="C45">
         <v>8</v>
       </c>
-      <c r="B28">
-        <v>0.16116536959631694</v>
-      </c>
-      <c r="C28" s="5">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="5"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30">
-        <v>0.13246554128353835</v>
-      </c>
-      <c r="C30" s="5">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31">
-        <v>0.10053047080811524</v>
-      </c>
-      <c r="C31" s="5">
-        <v>0.1</v>
+      <c r="D45" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46">
+        <v>34.523403428061599</v>
+      </c>
+      <c r="C46">
+        <v>35</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47">
+        <v>8.2937663365987877</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48">
+        <v>9.6265164197219288</v>
+      </c>
+      <c r="C48">
+        <v>10</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="5"/>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B50">
+        <v>10.463563838977411</v>
+      </c>
+      <c r="C50">
+        <v>10</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51">
+        <v>16.699053231758661</v>
+      </c>
+      <c r="C51">
+        <v>17</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52">
+        <v>20.222099150646397</v>
+      </c>
+      <c r="C52">
+        <v>20</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53">
+        <v>16.380729613957001</v>
+      </c>
+      <c r="C53">
+        <v>16</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Personality profile inference v0.3
</commit_message>
<xml_diff>
--- a/data/Average Emotion Statistics.xlsx
+++ b/data/Average Emotion Statistics.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="28">
   <si>
     <t>Dominance</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>2 each way</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of mentions / total words </t>
+  </si>
+  <si>
+    <t>% of positive words / tonal words</t>
   </si>
 </sst>
 </file>
@@ -160,8 +166,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -234,7 +254,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -257,6 +277,13 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -279,6 +306,13 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -608,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V53"/>
+  <dimension ref="A1:V85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1800,13 +1834,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:22">
       <c r="A49" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D49" s="5"/>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:22">
       <c r="A50" s="4" t="s">
         <v>17</v>
       </c>
@@ -1820,7 +1854,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:22">
       <c r="A51" s="4" t="s">
         <v>18</v>
       </c>
@@ -1834,7 +1868,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:22">
       <c r="A52" s="4" t="s">
         <v>19</v>
       </c>
@@ -1848,7 +1882,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:22">
       <c r="A53" s="4" t="s">
         <v>20</v>
       </c>
@@ -1860,6 +1894,663 @@
       </c>
       <c r="D53" s="5" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22">
+      <c r="A56" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22">
+      <c r="A57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57">
+        <v>11.226252158894599</v>
+      </c>
+      <c r="C57">
+        <v>6.3231850117096</v>
+      </c>
+      <c r="D57">
+        <v>8.5896076352067805</v>
+      </c>
+      <c r="E57">
+        <v>10.5084745762711</v>
+      </c>
+      <c r="F57">
+        <v>10.321489001691999</v>
+      </c>
+      <c r="G57">
+        <v>5.0259965337954897</v>
+      </c>
+      <c r="H57">
+        <v>8.3444592790387109</v>
+      </c>
+      <c r="I57">
+        <v>4.6469523234761603</v>
+      </c>
+      <c r="J57">
+        <v>6.5664160401002496</v>
+      </c>
+      <c r="K57">
+        <v>10.2564102564102</v>
+      </c>
+      <c r="L57">
+        <f>AVERAGE(B57:K57)</f>
+        <v>8.1809242816594896</v>
+      </c>
+      <c r="S57" s="7"/>
+      <c r="V57"/>
+    </row>
+    <row r="58" spans="1:22">
+      <c r="A58" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58">
+        <v>5.87219343696027</v>
+      </c>
+      <c r="C58">
+        <v>8.0562060889929707</v>
+      </c>
+      <c r="D58">
+        <v>3.9236479321314901</v>
+      </c>
+      <c r="E58">
+        <v>19.4350282485875</v>
+      </c>
+      <c r="F58">
+        <v>8.2910321489001699</v>
+      </c>
+      <c r="G58">
+        <v>10.2253032928942</v>
+      </c>
+      <c r="H58">
+        <v>12.483311081441901</v>
+      </c>
+      <c r="I58">
+        <v>11.5268557634278</v>
+      </c>
+      <c r="J58">
+        <v>3.7593984962406002</v>
+      </c>
+      <c r="K58">
+        <v>14.452214452214401</v>
+      </c>
+      <c r="L58">
+        <f t="shared" ref="L58:L69" si="2">AVERAGE(B58:K58)</f>
+        <v>9.8025190941791305</v>
+      </c>
+      <c r="S58" s="7"/>
+      <c r="V58"/>
+    </row>
+    <row r="59" spans="1:22">
+      <c r="A59" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59">
+        <v>4.6153846153846096</v>
+      </c>
+      <c r="C59">
+        <v>7.4074074074074003</v>
+      </c>
+      <c r="D59">
+        <v>9.8765432098765409</v>
+      </c>
+      <c r="E59">
+        <v>9.67741935483871</v>
+      </c>
+      <c r="F59">
+        <v>4.9180327868852398</v>
+      </c>
+      <c r="G59">
+        <v>20.689655172413701</v>
+      </c>
+      <c r="H59">
+        <v>8.7999999999999901</v>
+      </c>
+      <c r="I59">
+        <v>15.584415584415501</v>
+      </c>
+      <c r="J59">
+        <v>10.687022900763299</v>
+      </c>
+      <c r="K59">
+        <v>4.5454545454545396</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="2"/>
+        <v>9.680133557743952</v>
+      </c>
+      <c r="S59" s="7"/>
+      <c r="V59"/>
+    </row>
+    <row r="60" spans="1:22">
+      <c r="A60" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B60">
+        <v>18.4615384615384</v>
+      </c>
+      <c r="C60">
+        <v>2.2222222222222201</v>
+      </c>
+      <c r="D60">
+        <v>9.2592592592592595</v>
+      </c>
+      <c r="E60">
+        <v>4.3010752688171996</v>
+      </c>
+      <c r="F60">
+        <v>13.114754098360599</v>
+      </c>
+      <c r="G60">
+        <v>10.344827586206801</v>
+      </c>
+      <c r="H60">
+        <v>4</v>
+      </c>
+      <c r="I60">
+        <v>7.7922077922077904</v>
+      </c>
+      <c r="J60">
+        <v>6.1068702290076304</v>
+      </c>
+      <c r="K60">
+        <v>6.8181818181818103</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="2"/>
+        <v>8.24209367358017</v>
+      </c>
+      <c r="S60" s="7"/>
+      <c r="V60"/>
+    </row>
+    <row r="61" spans="1:22">
+      <c r="A61" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B61">
+        <v>4.6153846153846096</v>
+      </c>
+      <c r="C61">
+        <v>8.8888888888888893</v>
+      </c>
+      <c r="D61">
+        <v>14.1975308641975</v>
+      </c>
+      <c r="E61">
+        <v>6.4516129032257998</v>
+      </c>
+      <c r="F61">
+        <v>6.55737704918032</v>
+      </c>
+      <c r="G61">
+        <v>13.793103448275801</v>
+      </c>
+      <c r="H61">
+        <v>5.6</v>
+      </c>
+      <c r="I61">
+        <v>18.181818181818102</v>
+      </c>
+      <c r="J61">
+        <v>15.267175572518999</v>
+      </c>
+      <c r="K61">
+        <v>11.363636363636299</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="2"/>
+        <v>10.491652788712631</v>
+      </c>
+      <c r="S61" s="7"/>
+      <c r="V61"/>
+    </row>
+    <row r="62" spans="1:22">
+      <c r="A62" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62">
+        <v>26.1538461538461</v>
+      </c>
+      <c r="C62">
+        <v>10.370370370370299</v>
+      </c>
+      <c r="D62">
+        <v>14.1975308641975</v>
+      </c>
+      <c r="E62">
+        <v>16.129032258064498</v>
+      </c>
+      <c r="F62">
+        <v>18.032786885245901</v>
+      </c>
+      <c r="G62">
+        <v>10.344827586206801</v>
+      </c>
+      <c r="H62">
+        <v>25.6</v>
+      </c>
+      <c r="I62">
+        <v>14.285714285714199</v>
+      </c>
+      <c r="J62">
+        <v>12.9770992366412</v>
+      </c>
+      <c r="K62">
+        <v>18.181818181818102</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="2"/>
+        <v>16.627302582210461</v>
+      </c>
+      <c r="S62" s="7"/>
+      <c r="V62"/>
+    </row>
+    <row r="63" spans="1:22">
+      <c r="A63" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="S63" s="7"/>
+      <c r="V63"/>
+    </row>
+    <row r="64" spans="1:22">
+      <c r="A64" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B64">
+        <v>86.153846153846104</v>
+      </c>
+      <c r="C64">
+        <v>60.740740740740698</v>
+      </c>
+      <c r="D64">
+        <v>58.024691358024697</v>
+      </c>
+      <c r="E64">
+        <v>80.645161290322505</v>
+      </c>
+      <c r="F64">
+        <v>81.967213114754102</v>
+      </c>
+      <c r="G64">
+        <v>31.034482758620602</v>
+      </c>
+      <c r="H64">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="I64">
+        <v>50.649350649350602</v>
+      </c>
+      <c r="J64">
+        <v>67.1755725190839</v>
+      </c>
+      <c r="K64">
+        <v>75</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="2"/>
+        <v>65.699105858474312</v>
+      </c>
+      <c r="S64" s="7"/>
+      <c r="V64"/>
+    </row>
+    <row r="65" spans="1:22">
+      <c r="A65" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B65">
+        <v>5.87219343696027</v>
+      </c>
+      <c r="C65">
+        <v>8.0562060889929707</v>
+      </c>
+      <c r="D65">
+        <v>3.9236479321314901</v>
+      </c>
+      <c r="E65">
+        <v>19.4350282485875</v>
+      </c>
+      <c r="F65">
+        <v>8.2910321489001699</v>
+      </c>
+      <c r="G65">
+        <v>10.2253032928942</v>
+      </c>
+      <c r="H65">
+        <v>12.483311081441901</v>
+      </c>
+      <c r="I65">
+        <v>11.5268557634278</v>
+      </c>
+      <c r="J65">
+        <v>3.7593984962406002</v>
+      </c>
+      <c r="K65">
+        <v>14.452214452214401</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="2"/>
+        <v>9.8025190941791305</v>
+      </c>
+      <c r="S65" s="7"/>
+      <c r="V65"/>
+    </row>
+    <row r="66" spans="1:22">
+      <c r="A66" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B66">
+        <v>27.692307692307601</v>
+      </c>
+      <c r="C66">
+        <v>10.370370370370299</v>
+      </c>
+      <c r="D66">
+        <v>16.049382716049301</v>
+      </c>
+      <c r="E66">
+        <v>16.129032258064498</v>
+      </c>
+      <c r="F66">
+        <v>16.393442622950801</v>
+      </c>
+      <c r="G66">
+        <v>10.344827586206801</v>
+      </c>
+      <c r="H66">
+        <v>22.4</v>
+      </c>
+      <c r="I66">
+        <v>11.6883116883116</v>
+      </c>
+      <c r="J66">
+        <v>13.7404580152671</v>
+      </c>
+      <c r="K66">
+        <v>18.181818181818102</v>
+      </c>
+      <c r="L66">
+        <f t="shared" si="2"/>
+        <v>16.298995113134616</v>
+      </c>
+      <c r="S66" s="7"/>
+      <c r="V66"/>
+    </row>
+    <row r="67" spans="1:22">
+      <c r="A67" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67">
+        <v>40</v>
+      </c>
+      <c r="C67">
+        <v>12.592592592592499</v>
+      </c>
+      <c r="D67">
+        <v>22.839506172839499</v>
+      </c>
+      <c r="E67">
+        <v>16.129032258064498</v>
+      </c>
+      <c r="F67">
+        <v>19.672131147540899</v>
+      </c>
+      <c r="G67">
+        <v>10.344827586206801</v>
+      </c>
+      <c r="H67">
+        <v>28.799999999999901</v>
+      </c>
+      <c r="I67">
+        <v>11.6883116883116</v>
+      </c>
+      <c r="J67">
+        <v>20.610687022900699</v>
+      </c>
+      <c r="K67">
+        <v>18.181818181818102</v>
+      </c>
+      <c r="L67">
+        <f t="shared" si="2"/>
+        <v>20.085890665027449</v>
+      </c>
+      <c r="S67" s="7"/>
+      <c r="V67"/>
+    </row>
+    <row r="68" spans="1:22">
+      <c r="A68" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68">
+        <v>26.1538461538461</v>
+      </c>
+      <c r="C68">
+        <v>10.370370370370299</v>
+      </c>
+      <c r="D68">
+        <v>14.1975308641975</v>
+      </c>
+      <c r="E68">
+        <v>16.129032258064498</v>
+      </c>
+      <c r="F68">
+        <v>18.032786885245901</v>
+      </c>
+      <c r="G68">
+        <v>10.344827586206801</v>
+      </c>
+      <c r="H68">
+        <v>25.6</v>
+      </c>
+      <c r="I68">
+        <v>14.285714285714199</v>
+      </c>
+      <c r="J68">
+        <v>12.9770992366412</v>
+      </c>
+      <c r="K68">
+        <v>18.181818181818102</v>
+      </c>
+      <c r="L68">
+        <f t="shared" si="2"/>
+        <v>16.627302582210461</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22">
+      <c r="A69" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B69">
+        <v>4.6153846153846096</v>
+      </c>
+      <c r="C69">
+        <v>8.8888888888888893</v>
+      </c>
+      <c r="D69">
+        <v>14.1975308641975</v>
+      </c>
+      <c r="E69">
+        <v>6.4516129032257998</v>
+      </c>
+      <c r="F69">
+        <v>6.55737704918032</v>
+      </c>
+      <c r="G69">
+        <v>13.793103448275801</v>
+      </c>
+      <c r="H69">
+        <v>5.6</v>
+      </c>
+      <c r="I69">
+        <v>18.181818181818102</v>
+      </c>
+      <c r="J69">
+        <v>15.267175572518999</v>
+      </c>
+      <c r="K69">
+        <v>11.363636363636299</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="2"/>
+        <v>10.491652788712631</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22">
+      <c r="A72" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C72" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22">
+      <c r="A73" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B73">
+        <v>8.1809242816594896</v>
+      </c>
+      <c r="C73">
+        <v>8</v>
+      </c>
+      <c r="D73" s="5"/>
+    </row>
+    <row r="74" spans="1:22">
+      <c r="A74" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74">
+        <v>9.8025190941791305</v>
+      </c>
+      <c r="C74">
+        <v>10</v>
+      </c>
+      <c r="D74" s="5"/>
+    </row>
+    <row r="75" spans="1:22">
+      <c r="A75" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B75">
+        <v>9.6801335577439502</v>
+      </c>
+      <c r="C75">
+        <v>10</v>
+      </c>
+      <c r="D75" s="5"/>
+    </row>
+    <row r="76" spans="1:22">
+      <c r="A76" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B76">
+        <v>8.24209367358017</v>
+      </c>
+      <c r="C76">
+        <v>8</v>
+      </c>
+      <c r="D76" s="5"/>
+    </row>
+    <row r="77" spans="1:22">
+      <c r="A77" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B77">
+        <v>10.491652788712599</v>
+      </c>
+      <c r="C77">
+        <v>10</v>
+      </c>
+      <c r="D77" s="5"/>
+    </row>
+    <row r="78" spans="1:22">
+      <c r="A78" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B78">
+        <v>16.627302582210501</v>
+      </c>
+      <c r="C78">
+        <v>17</v>
+      </c>
+      <c r="D78" s="5"/>
+    </row>
+    <row r="79" spans="1:22">
+      <c r="A79" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D79" s="5"/>
+    </row>
+    <row r="80" spans="1:22">
+      <c r="A80" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B80">
+        <v>65.699105858474297</v>
+      </c>
+      <c r="C80">
+        <v>66</v>
+      </c>
+      <c r="D80" s="5"/>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B81">
+        <v>9.8025190941791305</v>
+      </c>
+      <c r="C81">
+        <v>10</v>
+      </c>
+      <c r="D81" s="5"/>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B82">
+        <v>16.298995113134598</v>
+      </c>
+      <c r="C82">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B83">
+        <v>20.085890665027399</v>
+      </c>
+      <c r="C83">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B84">
+        <v>16.627302582210501</v>
+      </c>
+      <c r="C84">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B85">
+        <v>10.491652788712599</v>
+      </c>
+      <c r="C85">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>